<commit_message>
rename default cover file
</commit_message>
<xml_diff>
--- a/tests/data/data with space/ncped with space.xlsx
+++ b/tests/data/data with space/ncped with space.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Word entries" sheetId="1" state="visible" r:id="rId2"/>
@@ -114,7 +114,7 @@
     <t xml:space="preserve">https://simsapa.github.io</t>
   </si>
   <si>
-    <t xml:space="preserve">cover.jpg</t>
+    <t xml:space="preserve">default_cover.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">NcpedDictionarySimsapa</t>
@@ -228,14 +228,14 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -313,7 +313,7 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix double first entry
</commit_message>
<xml_diff>
--- a/tests/data/data with space/ncped with space.xlsx
+++ b/tests/data/data with space/ncped with space.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Word entries" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,15 +38,6 @@
     <t xml:space="preserve">NCPED</t>
   </si>
   <si>
-    <t xml:space="preserve">ababa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the name of a hell, or place in Avīci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">masculine the name of a hell, or place in Avīci, where one suffers for an *ababa* of years.</t>
-  </si>
-  <si>
     <t xml:space="preserve">abbhantara</t>
   </si>
   <si>
@@ -78,6 +69,15 @@
     <t xml:space="preserve">pp mfn. distressed; grieved; pained (see *[aṭṭiyati](/define/aṭṭiyati)*)</t>
   </si>
   <si>
+    <t xml:space="preserve">cakkhuviññāṇa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cognizance by the sense-organ that is the eye.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">neuter cognizance by the sense\-organ that is the eye.</t>
+  </si>
+  <si>
     <t xml:space="preserve">cakkhuma</t>
   </si>
   <si>
@@ -90,13 +90,13 @@
 2. one who possess insight and vision; wise.</t>
   </si>
   <si>
-    <t xml:space="preserve">cakkhuviññāṇa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cognizance by the sense-organ that is the eye.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">neuter cognizance by the sense\-organ that is the eye.</t>
+    <t xml:space="preserve">ababa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the name of a hell, or place in Avīci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">masculine the name of a hell, or place in Avīci, where one suffers for an *ababa* of years.</t>
   </si>
   <si>
     <t xml:space="preserve">title</t>
@@ -258,8 +258,8 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -283,7 +283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -293,11 +293,11 @@
       <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
@@ -321,7 +321,7 @@
       <c r="C4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -385,7 +385,7 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -454,7 +454,8 @@
       <c r="H2" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="2" t="b">
+      <c r="I2" s="2" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J2" s="2" t="n">

</xml_diff>

<commit_message>
default value for missing fields
</commit_message>
<xml_diff>
--- a/tests/data/data with space/ncped with space.xlsx
+++ b/tests/data/data with space/ncped with space.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t xml:space="preserve">dict_label</t>
   </si>
@@ -32,6 +32,12 @@
     <t xml:space="preserve">summary</t>
   </si>
   <si>
+    <t xml:space="preserve">grammar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">synonyms</t>
+  </si>
+  <si>
     <t xml:space="preserve">definition_md</t>
   </si>
   <si>
@@ -44,8 +50,10 @@
     <t xml:space="preserve">interior, internal; being within, included in</t>
   </si>
   <si>
-    <t xml:space="preserve">mfn. &amp; neuter
-1. (mfn.) interior, internal; being within, included in, among; belonging to one ‘s house, personal, intimate.
+    <t xml:space="preserve">mfn. &amp; neuter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. (mfn.) interior, internal; being within, included in, among; belonging to one ‘s house, personal, intimate.
 2. (n.)
    1. intermediate space, interval; the inside, interior.
    2. a measure of length (= 28 hatthas).</t>
@@ -57,7 +65,7 @@
     <t xml:space="preserve">in the open air, in the open.</t>
   </si>
   <si>
-    <t xml:space="preserve">ind. in the open air, in the open.</t>
+    <t xml:space="preserve">ind.</t>
   </si>
   <si>
     <t xml:space="preserve">aṭṭita</t>
@@ -66,7 +74,10 @@
     <t xml:space="preserve">distressed; grieved; pained (see aṭṭiyati)</t>
   </si>
   <si>
-    <t xml:space="preserve">pp mfn. distressed; grieved; pained (see *[aṭṭiyati](/define/aṭṭiyati)*)</t>
+    <t xml:space="preserve">pp mfn. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">distressed; grieved; pained (see *[aṭṭiyati](/define/aṭṭiyati)*)</t>
   </si>
   <si>
     <t xml:space="preserve">cakkhuviññāṇa</t>
@@ -75,7 +86,10 @@
     <t xml:space="preserve">cognizance by the sense-organ that is the eye.</t>
   </si>
   <si>
-    <t xml:space="preserve">neuter cognizance by the sense\-organ that is the eye.</t>
+    <t xml:space="preserve">neuter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cognizance by the sense\-organ that is the eye.</t>
   </si>
   <si>
     <t xml:space="preserve">cakkhuma</t>
@@ -84,9 +98,10 @@
     <t xml:space="preserve">possessing eyes, gifted with sight;</t>
   </si>
   <si>
-    <t xml:space="preserve">cakkhuma(t)
-mfn. &amp; masculine
-1. possessing eyes, gifted with sight; (one) who has eyes, who can see; one who has the gift of sight.
+    <t xml:space="preserve">mfn. &amp; masculine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. possessing eyes, gifted with sight; (one) who has eyes, who can see; one who has the gift of sight.
 2. one who possess insight and vision; wise.</t>
   </si>
   <si>
@@ -96,7 +111,10 @@
     <t xml:space="preserve">the name of a hell, or place in Avīci</t>
   </si>
   <si>
-    <t xml:space="preserve">masculine the name of a hell, or place in Avīci, where one suffers for an *ababa* of years.</t>
+    <t xml:space="preserve">masculine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the name of a hell, or place in Avīci, where one suffers for an *ababa* of years.</t>
   </si>
   <si>
     <t xml:space="preserve">title</t>
@@ -226,8 +244,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,17 +278,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="51.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -282,89 +306,113 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>4</v>
-      </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -396,73 +444,73 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="I2" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="J2" s="3" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="K2" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>